<commit_message>
sbde dates, english registration headers
</commit_message>
<xml_diff>
--- a/owlcms/src/main/resources/templates/registration/SBDE.xlsx
+++ b/owlcms/src/main/resources/templates/registration/SBDE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lamyj\git\owlcms4\owlcms\src\main\resources\templates\registration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5658871-65BB-4DEB-8BF4-F7B10A6093B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD56DCD-43E8-4575-803B-746DAE481837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23475" yWindow="1770" windowWidth="20715" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Athletes" sheetId="1" r:id="rId1"/>
@@ -222,9 +222,6 @@
     <t>${l.club}</t>
   </si>
   <si>
-    <t>${l.formattedBirth}</t>
-  </si>
-  <si>
     <t>${l.snatch1Declaration}</t>
   </si>
   <si>
@@ -493,6 +490,9 @@
   </si>
   <si>
     <t>${l.subCategory}</t>
+  </si>
+  <si>
+    <t>${l.isoBirth}</t>
   </si>
 </sst>
 </file>
@@ -1384,17 +1384,17 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
   <cellStyles count="36">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1434,87 +1434,7 @@
     <cellStyle name="Title" xfId="34" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="35" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="92">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="34"/>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="34"/>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="34"/>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="34"/>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="34"/>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="34"/>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="34"/>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="34"/>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="34"/>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="34"/>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="89">
     <dxf>
       <font>
         <b/>
@@ -1783,6 +1703,62 @@
           <color theme="4" tint="0.499984740745262"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -2154,7 +2130,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Jean-François Lamy" refreshedDate="45333.666685879631" createdVersion="8" refreshedVersion="8" recordCount="20" xr:uid="{00000000-000A-0000-FFFF-FFFF09000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Jean-François Lamy" refreshedDate="45393.588059027781" createdVersion="8" refreshedVersion="8" recordCount="20" xr:uid="{00000000-000A-0000-FFFF-FFFF09000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:G600" sheet="Group Data"/>
   </cacheSource>
@@ -2655,13 +2631,13 @@
     <i/>
   </colItems>
   <formats count="41">
-    <format dxfId="91">
+    <format dxfId="88">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="90">
+    <format dxfId="87">
       <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="89">
+    <format dxfId="86">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="6" count="1">
@@ -2670,7 +2646,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="88">
+    <format dxfId="85">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="6" count="1" countASubtotal="1">
@@ -2679,7 +2655,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="87">
+    <format dxfId="84">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="6" count="1">
@@ -2688,7 +2664,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="86">
+    <format dxfId="83">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="6" count="1" countASubtotal="1">
@@ -2697,7 +2673,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="85">
+    <format dxfId="82">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="6" count="1">
@@ -2706,7 +2682,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="84">
+    <format dxfId="81">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="6" count="1" countASubtotal="1">
@@ -2715,7 +2691,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="83">
+    <format dxfId="80">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="6" count="1">
@@ -2724,7 +2700,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="82">
+    <format dxfId="79">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="6" count="1" countASubtotal="1">
@@ -2733,7 +2709,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="81">
+    <format dxfId="78">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="6" count="1">
@@ -2742,7 +2718,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="80">
+    <format dxfId="77">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="6" count="1" countASubtotal="1">
@@ -2751,7 +2727,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="79">
+    <format dxfId="76">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="6" count="1">
@@ -2760,7 +2736,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="78">
+    <format dxfId="75">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="6" count="1" countASubtotal="1">
@@ -2769,7 +2745,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="77">
+    <format dxfId="74">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="6" count="1">
@@ -2778,7 +2754,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="76">
+    <format dxfId="73">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="6" count="1" countASubtotal="1">
@@ -2787,7 +2763,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="75">
+    <format dxfId="72">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="6" count="1">
@@ -2796,7 +2772,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="74">
+    <format dxfId="71">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="6" count="1" countASubtotal="1">
@@ -2805,7 +2781,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="73">
+    <format dxfId="70">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="6" count="1">
@@ -2814,7 +2790,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="72">
+    <format dxfId="69">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="6" count="1" countASubtotal="1">
@@ -2823,7 +2799,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="71">
+    <format dxfId="68">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="6" count="1">
@@ -2832,7 +2808,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="70">
+    <format dxfId="67">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="6" count="1" countASubtotal="1">
@@ -2841,7 +2817,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="69">
+    <format dxfId="66">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="6" count="1">
@@ -2850,7 +2826,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="68">
+    <format dxfId="65">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="6" count="1" countASubtotal="1">
@@ -2859,7 +2835,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="67">
+    <format dxfId="64">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="6" count="1">
@@ -2868,7 +2844,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="66">
+    <format dxfId="63">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="6" count="1" countASubtotal="1">
@@ -2877,7 +2853,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="65">
+    <format dxfId="62">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="6" count="1">
@@ -2886,7 +2862,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="64">
+    <format dxfId="61">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="6" count="1" countASubtotal="1">
@@ -2895,7 +2871,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="63">
+    <format dxfId="60">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="6" count="1">
@@ -2904,7 +2880,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="62">
+    <format dxfId="59">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="6" count="1" countASubtotal="1">
@@ -2913,7 +2889,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="61">
+    <format dxfId="58">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="6" count="1">
@@ -2922,7 +2898,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="60">
+    <format dxfId="57">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="6" count="1" countASubtotal="1">
@@ -2931,7 +2907,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="59">
+    <format dxfId="56">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="6" count="1">
@@ -2940,7 +2916,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="58">
+    <format dxfId="55">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="6" count="1" countASubtotal="1">
@@ -2949,7 +2925,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="57">
+    <format dxfId="54">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="6" count="1">
@@ -2958,7 +2934,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="56">
+    <format dxfId="53">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="6" count="1" countASubtotal="1">
@@ -2967,19 +2943,19 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="55">
+    <format dxfId="52">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="54">
+    <format dxfId="51">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" offset="A1" fieldPosition="0"/>
     </format>
-    <format dxfId="53">
+    <format dxfId="50">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" offset="A1" fieldPosition="0"/>
     </format>
-    <format dxfId="52">
+    <format dxfId="49">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" offset="A1" fieldPosition="0"/>
     </format>
-    <format dxfId="51">
+    <format dxfId="48">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
@@ -3287,7 +3263,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" workbookViewId="0">
       <pane xSplit="5" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A9" sqref="A9"/>
+      <selection pane="topRight" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -3311,7 +3287,7 @@
   <sheetData>
     <row r="1" spans="1:242" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="24"/>
@@ -3319,7 +3295,7 @@
         <v>12</v>
       </c>
       <c r="F1" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G1" s="13"/>
       <c r="H1" s="13"/>
@@ -3329,9 +3305,9 @@
         <v>15</v>
       </c>
       <c r="M1" s="67" t="s">
-        <v>42</v>
-      </c>
-      <c r="N1" s="73"/>
+        <v>41</v>
+      </c>
+      <c r="N1" s="70"/>
       <c r="P1" s="22"/>
       <c r="Q1" s="22"/>
       <c r="R1" s="22"/>
@@ -3339,14 +3315,14 @@
     </row>
     <row r="2" spans="1:242" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" s="19"/>
       <c r="E2" s="26" t="s">
         <v>16</v>
       </c>
       <c r="F2" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G2" s="13"/>
       <c r="H2" s="13"/>
@@ -3356,14 +3332,14 @@
     </row>
     <row r="3" spans="1:242" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" s="21"/>
       <c r="E3" s="26" t="s">
         <v>13</v>
       </c>
       <c r="F3" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
@@ -3374,14 +3350,14 @@
     </row>
     <row r="4" spans="1:242" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" s="20"/>
       <c r="E4" s="26" t="s">
         <v>14</v>
       </c>
       <c r="F4" s="27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G4" s="13"/>
       <c r="H4" s="13"/>
@@ -3392,40 +3368,40 @@
     </row>
     <row r="5" spans="1:242" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:242" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="72" t="s">
-        <v>73</v>
-      </c>
-      <c r="B6" s="72"/>
-      <c r="C6" s="72"/>
-      <c r="D6" s="72"/>
-      <c r="E6" s="72"/>
-      <c r="F6" s="72"/>
-      <c r="G6" s="72"/>
-      <c r="H6" s="72"/>
-      <c r="I6" s="72"/>
-      <c r="J6" s="72"/>
-      <c r="K6" s="72"/>
-      <c r="L6" s="72"/>
-      <c r="M6" s="72"/>
+      <c r="A6" s="71" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="71"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="71"/>
+      <c r="H6" s="71"/>
+      <c r="I6" s="71"/>
+      <c r="J6" s="71"/>
+      <c r="K6" s="71"/>
+      <c r="L6" s="71"/>
+      <c r="M6" s="71"/>
       <c r="N6" s="69"/>
       <c r="O6" s="69"/>
     </row>
     <row r="7" spans="1:242" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="72" t="s">
+      <c r="A7" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="72"/>
-      <c r="C7" s="72"/>
-      <c r="D7" s="72"/>
-      <c r="E7" s="72"/>
-      <c r="F7" s="72"/>
-      <c r="G7" s="72"/>
-      <c r="H7" s="72"/>
-      <c r="I7" s="72"/>
-      <c r="J7" s="72"/>
-      <c r="K7" s="72"/>
-      <c r="L7" s="72"/>
-      <c r="M7" s="72"/>
+      <c r="B7" s="71"/>
+      <c r="C7" s="71"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="71"/>
+      <c r="G7" s="71"/>
+      <c r="H7" s="71"/>
+      <c r="I7" s="71"/>
+      <c r="J7" s="71"/>
+      <c r="K7" s="71"/>
+      <c r="L7" s="71"/>
+      <c r="M7" s="71"/>
       <c r="N7" s="69"/>
       <c r="O7" s="69"/>
     </row>
@@ -3475,7 +3451,7 @@
         <v>6</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K9" s="10" t="s">
         <v>4</v>
@@ -3484,25 +3460,25 @@
         <v>3</v>
       </c>
       <c r="M9" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N9" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O9" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P9" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q9" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="Q9" s="10" t="s">
+      <c r="R9" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="R9" s="10" t="s">
+      <c r="S9" s="10" t="s">
         <v>110</v>
-      </c>
-      <c r="S9" s="10" t="s">
-        <v>111</v>
       </c>
       <c r="T9" s="10" t="s">
         <v>1</v>
@@ -3511,7 +3487,7 @@
         <v>2</v>
       </c>
       <c r="V9" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:242" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3775,55 +3751,55 @@
         <v>27</v>
       </c>
       <c r="F11" s="46" t="s">
-        <v>28</v>
+        <v>118</v>
       </c>
       <c r="G11" s="30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H11" s="37" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I11" s="41" t="s">
         <v>26</v>
       </c>
       <c r="J11" s="44" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K11" s="42" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L11" s="44" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M11" s="45" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N11" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="O11" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="O11" s="45" t="s">
-        <v>86</v>
-      </c>
       <c r="P11" s="45" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="Q11" s="45" t="s">
+        <v>111</v>
+      </c>
+      <c r="R11" s="45" t="s">
         <v>112</v>
       </c>
-      <c r="R11" s="45" t="s">
+      <c r="S11" s="45" t="s">
         <v>113</v>
       </c>
-      <c r="S11" s="45" t="s">
+      <c r="T11" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="U11" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="V11" s="45" t="s">
         <v>114</v>
-      </c>
-      <c r="T11" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="U11" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="V11" s="45" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:242" x14ac:dyDescent="0.25">
@@ -7381,52 +7357,37 @@
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="C11:F11">
-    <cfRule type="expression" dxfId="9" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="10" stopIfTrue="1">
       <formula>AND((#REF!),#REF!,#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13:F33">
-    <cfRule type="expression" dxfId="8" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="8" stopIfTrue="1">
+      <formula>AND((#REF!),#REF!,#REF!)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C34:F54">
+    <cfRule type="expression" dxfId="45" priority="6" stopIfTrue="1">
+      <formula>AND((#REF!),#REF!,#REF!)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C55:F75">
+    <cfRule type="expression" dxfId="44" priority="5" stopIfTrue="1">
+      <formula>AND((#REF!),#REF!,#REF!)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C76:F159">
+    <cfRule type="expression" dxfId="43" priority="1" stopIfTrue="1">
       <formula>AND((#REF!),#REF!,#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G11">
-    <cfRule type="expression" dxfId="7" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="9" stopIfTrue="1">
       <formula>AND((#REF!),#REF!,#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G13:G159">
-    <cfRule type="expression" dxfId="6" priority="7" stopIfTrue="1">
-      <formula>AND((#REF!),#REF!,#REF!)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C34:F54">
-    <cfRule type="expression" dxfId="5" priority="6" stopIfTrue="1">
-      <formula>AND((#REF!),#REF!,#REF!)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C55:F75">
-    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
-      <formula>AND((#REF!),#REF!,#REF!)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C76:F96">
-    <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
-      <formula>AND((#REF!),#REF!,#REF!)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C97:F117">
-    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
-      <formula>AND((#REF!),#REF!,#REF!)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C118:F138">
-    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
-      <formula>AND((#REF!),#REF!,#REF!)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C139:F159">
-    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="7" stopIfTrue="1">
       <formula>AND((#REF!),#REF!,#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7460,85 +7421,85 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
     </row>
     <row r="2" spans="1:22" s="39" customFormat="1" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="I2" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="J2" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="K2" s="39" t="s">
+        <v>74</v>
+      </c>
+      <c r="L2" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="39" t="s">
-        <v>88</v>
-      </c>
-      <c r="D2" s="39" t="s">
-        <v>80</v>
-      </c>
-      <c r="E2" s="39" t="s">
-        <v>81</v>
-      </c>
-      <c r="F2" s="39" t="s">
-        <v>78</v>
-      </c>
-      <c r="G2" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="H2" s="39" t="s">
-        <v>76</v>
-      </c>
-      <c r="I2" s="39" t="s">
-        <v>77</v>
-      </c>
-      <c r="J2" s="39" t="s">
-        <v>92</v>
-      </c>
-      <c r="K2" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="L2" s="39" t="s">
+      <c r="M2" s="39" t="s">
+        <v>89</v>
+      </c>
+      <c r="N2" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="M2" s="39" t="s">
-        <v>90</v>
-      </c>
-      <c r="N2" s="39" t="s">
+      <c r="O2" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="P2" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="O2" s="39" t="s">
+      <c r="Q2" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="P2" s="39" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q2" s="39" t="s">
+      <c r="R2" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="R2" s="39" t="s">
+      <c r="S2" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="S2" s="39" t="s">
+      <c r="T2" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="T2" s="39" t="s">
+      <c r="U2" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="U2" s="39" t="s">
-        <v>72</v>
-      </c>
       <c r="V2" s="39" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D3"/>
       <c r="E3" s="1"/>
@@ -7547,70 +7508,70 @@
     </row>
     <row r="4" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D4" s="40" t="s">
+      <c r="E4" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="40" t="s">
+      <c r="F4" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="M4" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="N4" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="M4" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="N4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="R4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="V4" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
@@ -7656,11 +7617,11 @@
   <sheetData>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="50" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="71"/>
+      <c r="A3" s="73"/>
       <c r="B3" s="51"/>
       <c r="C3" s="51"/>
       <c r="D3" s="51"/>
@@ -7675,22 +7636,22 @@
     </row>
     <row r="4" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="64" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" s="52" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="52" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" s="52" t="s">
         <v>95</v>
       </c>
-      <c r="B4" s="52" t="s">
-        <v>98</v>
-      </c>
-      <c r="C4" s="52" t="s">
-        <v>100</v>
-      </c>
-      <c r="D4" s="52" t="s">
+      <c r="E4" s="52" t="s">
         <v>96</v>
       </c>
-      <c r="E4" s="52" t="s">
-        <v>97</v>
-      </c>
       <c r="F4" s="52" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G4" s="57"/>
       <c r="H4" s="56"/>
@@ -7701,22 +7662,22 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="63" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5" s="53" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="53" t="s">
-        <v>45</v>
-      </c>
       <c r="D5" s="53" t="s">
+        <v>102</v>
+      </c>
+      <c r="E5" s="53" t="s">
         <v>103</v>
       </c>
-      <c r="E5" s="53" t="s">
-        <v>104</v>
-      </c>
       <c r="F5" s="53" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G5" s="53"/>
       <c r="H5" s="54"/>
@@ -7727,22 +7688,22 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="63" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B6" s="53" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="53" t="s">
-        <v>45</v>
-      </c>
       <c r="D6" s="53" t="s">
+        <v>102</v>
+      </c>
+      <c r="E6" s="53" t="s">
         <v>103</v>
       </c>
-      <c r="E6" s="53" t="s">
-        <v>104</v>
-      </c>
       <c r="F6" s="53" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G6" s="57"/>
       <c r="H6" s="56"/>
@@ -7753,22 +7714,22 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="63" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B7" s="53" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="53" t="s">
-        <v>45</v>
-      </c>
       <c r="D7" s="53" t="s">
+        <v>102</v>
+      </c>
+      <c r="E7" s="53" t="s">
         <v>103</v>
       </c>
-      <c r="E7" s="53" t="s">
-        <v>104</v>
-      </c>
       <c r="F7" s="53" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G7" s="57"/>
       <c r="H7" s="56"/>
@@ -7779,22 +7740,22 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="63" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B8" s="53" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="53" t="s">
-        <v>45</v>
-      </c>
       <c r="D8" s="53" t="s">
+        <v>102</v>
+      </c>
+      <c r="E8" s="53" t="s">
         <v>103</v>
       </c>
-      <c r="E8" s="53" t="s">
-        <v>104</v>
-      </c>
       <c r="F8" s="53" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G8" s="57"/>
       <c r="H8" s="56"/>
@@ -7805,22 +7766,22 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="63" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B9" s="53" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="53" t="s">
-        <v>45</v>
-      </c>
       <c r="D9" s="53" t="s">
+        <v>102</v>
+      </c>
+      <c r="E9" s="53" t="s">
         <v>103</v>
       </c>
-      <c r="E9" s="53" t="s">
-        <v>104</v>
-      </c>
       <c r="F9" s="53" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G9" s="57"/>
       <c r="H9" s="56"/>
@@ -7831,22 +7792,22 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="63" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B10" s="53" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="53" t="s">
-        <v>45</v>
-      </c>
       <c r="D10" s="53" t="s">
+        <v>102</v>
+      </c>
+      <c r="E10" s="53" t="s">
         <v>103</v>
       </c>
-      <c r="E10" s="53" t="s">
-        <v>104</v>
-      </c>
       <c r="F10" s="53" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G10" s="57"/>
       <c r="H10" s="56"/>
@@ -7857,22 +7818,22 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="63" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B11" s="53" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="53" t="s">
-        <v>45</v>
-      </c>
       <c r="D11" s="53" t="s">
+        <v>102</v>
+      </c>
+      <c r="E11" s="53" t="s">
         <v>103</v>
       </c>
-      <c r="E11" s="53" t="s">
-        <v>104</v>
-      </c>
       <c r="F11" s="53" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G11" s="57"/>
       <c r="H11" s="56"/>
@@ -7883,22 +7844,22 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="63" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B12" s="53" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="53" t="s">
-        <v>45</v>
-      </c>
       <c r="D12" s="53" t="s">
+        <v>102</v>
+      </c>
+      <c r="E12" s="53" t="s">
         <v>103</v>
       </c>
-      <c r="E12" s="53" t="s">
-        <v>104</v>
-      </c>
       <c r="F12" s="53" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G12" s="57"/>
       <c r="H12" s="56"/>
@@ -7909,22 +7870,22 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="63" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B13" s="53" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="53" t="s">
-        <v>45</v>
-      </c>
       <c r="D13" s="53" t="s">
+        <v>102</v>
+      </c>
+      <c r="E13" s="53" t="s">
         <v>103</v>
       </c>
-      <c r="E13" s="53" t="s">
-        <v>104</v>
-      </c>
       <c r="F13" s="53" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G13" s="57"/>
       <c r="H13" s="56"/>
@@ -7935,22 +7896,22 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="63" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B14" s="53" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="53" t="s">
-        <v>45</v>
-      </c>
       <c r="D14" s="53" t="s">
+        <v>102</v>
+      </c>
+      <c r="E14" s="53" t="s">
         <v>103</v>
       </c>
-      <c r="E14" s="53" t="s">
-        <v>104</v>
-      </c>
       <c r="F14" s="53" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G14" s="57"/>
       <c r="H14" s="56"/>
@@ -7961,22 +7922,22 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="63" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B15" s="53" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="53" t="s">
-        <v>45</v>
-      </c>
       <c r="D15" s="53" t="s">
+        <v>102</v>
+      </c>
+      <c r="E15" s="53" t="s">
         <v>103</v>
       </c>
-      <c r="E15" s="53" t="s">
-        <v>104</v>
-      </c>
       <c r="F15" s="53" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G15" s="57"/>
       <c r="H15" s="56"/>
@@ -7987,22 +7948,22 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="63" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B16" s="53" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="53" t="s">
-        <v>45</v>
-      </c>
       <c r="D16" s="53" t="s">
+        <v>102</v>
+      </c>
+      <c r="E16" s="53" t="s">
         <v>103</v>
       </c>
-      <c r="E16" s="53" t="s">
-        <v>104</v>
-      </c>
       <c r="F16" s="53" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G16" s="57"/>
       <c r="H16" s="56"/>
@@ -8013,22 +7974,22 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="63" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B17" s="53" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="53" t="s">
-        <v>45</v>
-      </c>
       <c r="D17" s="53" t="s">
+        <v>102</v>
+      </c>
+      <c r="E17" s="53" t="s">
         <v>103</v>
       </c>
-      <c r="E17" s="53" t="s">
-        <v>104</v>
-      </c>
       <c r="F17" s="53" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G17" s="57"/>
       <c r="H17" s="56"/>
@@ -8039,22 +8000,22 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="63" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B18" s="53" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="53" t="s">
-        <v>45</v>
-      </c>
       <c r="D18" s="53" t="s">
+        <v>102</v>
+      </c>
+      <c r="E18" s="53" t="s">
         <v>103</v>
       </c>
-      <c r="E18" s="53" t="s">
-        <v>104</v>
-      </c>
       <c r="F18" s="53" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G18" s="57"/>
       <c r="H18" s="56"/>
@@ -8065,22 +8026,22 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="63" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B19" s="53" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="53" t="s">
-        <v>45</v>
-      </c>
       <c r="D19" s="53" t="s">
+        <v>102</v>
+      </c>
+      <c r="E19" s="53" t="s">
         <v>103</v>
       </c>
-      <c r="E19" s="53" t="s">
-        <v>104</v>
-      </c>
       <c r="F19" s="53" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G19" s="57"/>
       <c r="H19" s="56"/>
@@ -8091,22 +8052,22 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="63" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B20" s="53" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="53" t="s">
-        <v>45</v>
-      </c>
       <c r="D20" s="53" t="s">
+        <v>102</v>
+      </c>
+      <c r="E20" s="53" t="s">
         <v>103</v>
       </c>
-      <c r="E20" s="53" t="s">
-        <v>104</v>
-      </c>
       <c r="F20" s="53" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G20" s="57"/>
       <c r="H20" s="56"/>
@@ -8117,22 +8078,22 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="63" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B21" s="53" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="53" t="s">
-        <v>45</v>
-      </c>
       <c r="D21" s="53" t="s">
+        <v>102</v>
+      </c>
+      <c r="E21" s="53" t="s">
         <v>103</v>
       </c>
-      <c r="E21" s="53" t="s">
-        <v>104</v>
-      </c>
       <c r="F21" s="53" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G21" s="57"/>
       <c r="H21" s="56"/>
@@ -8143,7 +8104,7 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="65" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B22" s="66"/>
       <c r="C22" s="66"/>
@@ -8236,54 +8197,54 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="39" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B1" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" s="39" t="s">
         <v>100</v>
       </c>
-      <c r="C1" s="39" t="s">
-        <v>101</v>
-      </c>
       <c r="D1" s="47" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="47" t="s">
         <v>96</v>
       </c>
-      <c r="E1" s="47" t="s">
-        <v>97</v>
-      </c>
       <c r="F1" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" s="39" t="s">
         <v>94</v>
-      </c>
-      <c r="G1" s="39" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E2" s="49"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D3" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="E3" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="E3" s="49" t="s">
-        <v>104</v>
-      </c>
       <c r="F3" s="39" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H3" s="14"/>
       <c r="I3"/>
@@ -8291,25 +8252,25 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D4" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="E4" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="E4" s="49" t="s">
-        <v>104</v>
-      </c>
       <c r="F4" s="39" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H4" s="14"/>
       <c r="I4"/>
@@ -8317,25 +8278,25 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D5" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="E5" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="E5" s="49" t="s">
-        <v>104</v>
-      </c>
       <c r="F5" s="39" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H5" s="14"/>
       <c r="I5"/>
@@ -8343,25 +8304,25 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="C6" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D6" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="E6" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="E6" s="49" t="s">
-        <v>104</v>
-      </c>
       <c r="F6" s="39" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H6" s="14"/>
       <c r="I6"/>
@@ -8369,25 +8330,25 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="C7" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D7" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="E7" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="E7" s="49" t="s">
-        <v>104</v>
-      </c>
       <c r="F7" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="H7" s="14"/>
       <c r="I7"/>
@@ -8395,25 +8356,25 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="C8" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D8" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="E8" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="E8" s="49" t="s">
-        <v>104</v>
-      </c>
       <c r="F8" s="39" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H8" s="14"/>
       <c r="I8"/>
@@ -8421,25 +8382,25 @@
     </row>
     <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="C9" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D9" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="E9" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="E9" s="49" t="s">
-        <v>104</v>
-      </c>
       <c r="F9" s="39" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H9" s="14"/>
       <c r="I9"/>
@@ -8447,25 +8408,25 @@
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="C10" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D10" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="E10" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="F10" s="39" t="s">
         <v>89</v>
       </c>
-      <c r="D10" s="49" t="s">
-        <v>103</v>
-      </c>
-      <c r="E10" s="49" t="s">
-        <v>104</v>
-      </c>
-      <c r="F10" s="39" t="s">
+      <c r="G10" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="H10" s="14"/>
       <c r="I10"/>
@@ -8473,25 +8434,25 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="C11" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D11" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="E11" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="E11" s="49" t="s">
-        <v>104</v>
-      </c>
       <c r="F11" s="39" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H11" s="14"/>
       <c r="I11"/>
@@ -8499,25 +8460,25 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="C12" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D12" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="E12" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="E12" s="49" t="s">
-        <v>104</v>
-      </c>
       <c r="F12" s="39" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H12" s="14"/>
       <c r="I12"/>
@@ -8525,25 +8486,25 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="C13" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D13" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="E13" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="E13" s="49" t="s">
-        <v>104</v>
-      </c>
       <c r="F13" s="39" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H13" s="14"/>
       <c r="I13"/>
@@ -8551,25 +8512,25 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="C14" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D14" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="E14" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="E14" s="49" t="s">
-        <v>104</v>
-      </c>
       <c r="F14" s="39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H14" s="14"/>
       <c r="I14"/>
@@ -8577,25 +8538,25 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="C15" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D15" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="E15" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="E15" s="49" t="s">
-        <v>104</v>
-      </c>
       <c r="F15" s="39" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H15" s="14"/>
       <c r="I15"/>
@@ -8603,25 +8564,25 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="C16" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D16" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="E16" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="E16" s="49" t="s">
-        <v>104</v>
-      </c>
       <c r="F16" s="39" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H16" s="14"/>
       <c r="I16"/>
@@ -8629,25 +8590,25 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="C17" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D17" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="E17" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="E17" s="49" t="s">
-        <v>104</v>
-      </c>
       <c r="F17" s="39" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H17" s="14"/>
       <c r="I17"/>
@@ -8655,25 +8616,25 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="C18" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D18" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="E18" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="E18" s="49" t="s">
-        <v>104</v>
-      </c>
       <c r="F18" s="39" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H18" s="14"/>
       <c r="I18"/>
@@ -8681,25 +8642,25 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="C19" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D19" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="E19" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="E19" s="49" t="s">
-        <v>104</v>
-      </c>
       <c r="F19" s="39" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H19" s="14"/>
       <c r="J19"/>
@@ -8711,7 +8672,7 @@
     </row>
     <row r="602" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A602" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SBDE did not export sessions
</commit_message>
<xml_diff>
--- a/owlcms/src/main/resources/templates/registration/SBDE.xlsx
+++ b/owlcms/src/main/resources/templates/registration/SBDE.xlsx
@@ -5,10 +5,10 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\usaw-owlcms\local\templates\registration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lamyj\git\owlcms4\owlcms\src\main\resources\templates\registration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCFB7A2F-AD24-4E50-B266-94970C65111B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCD68300-3437-4B1B-829D-7933A5A3B409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -121,7 +121,7 @@
   </definedNames>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="19" r:id="rId6"/>
+    <pivotCache cacheId="9" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -193,8 +193,93 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Jean-François Lamy</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{AD0D4021-F377-4613-9645-B425EF7B630B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>jx:area(lastCell="V3")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{F484B613-7CE3-4869-B306-F7C6BC24CCE1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>jx:each(items="groups" var="g" lastCell="V3")</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Jean-François Lamy</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{BAA11956-0102-451B-9633-F65EE62A5BBD}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">jx:area(lastCell="G18")
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{1A4E3F3C-9CC0-456B-A589-0F75151D2499}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">jx:each(items="groups" var="g" lastCell="G18")
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="116">
   <si>
     <t>M/F</t>
   </si>
@@ -256,9 +341,6 @@
     <t>${t.get("Registration.groupsOverwrite")}</t>
   </si>
   <si>
-    <t>&lt;/jx:forEach&gt;</t>
-  </si>
-  <si>
     <t>${l.membership}</t>
   </si>
   <si>
@@ -317,9 +399,6 @@
   </si>
   <si>
     <t>${competition.competitionDateAsDate}</t>
-  </si>
-  <si>
-    <t>&lt;jx:forEach items="${groups}" var="g" varStatus="index"&gt;</t>
   </si>
   <si>
     <t>${g.name}</t>
@@ -2191,23 +2270,23 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Jean-François Lamy" refreshedDate="45527.713239699071" createdVersion="8" refreshedVersion="8" recordCount="20" xr:uid="{00000000-000A-0000-FFFF-FFFF09000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Jean-François Lamy" refreshedDate="45532.984339236114" createdVersion="8" refreshedVersion="8" recordCount="18" xr:uid="{00000000-000A-0000-FFFF-FFFF09000000}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:G600" sheet="Group Data"/>
+    <worksheetSource ref="A1:G598" sheet="Group Data"/>
   </cacheSource>
   <cacheFields count="7">
     <cacheField name="Group" numFmtId="0">
       <sharedItems containsBlank="1" count="4">
-        <s v="&lt;jx:forEach items=&quot;${groups}&quot; var=&quot;g&quot; varStatus=&quot;index&quot;&gt;"/>
         <s v="${g.name}"/>
-        <s v="&lt;/jx:forEach&gt;"/>
         <m/>
+        <s v="&lt;jx:forEach items=&quot;${groups}&quot; var=&quot;g&quot; varStatus=&quot;index&quot;&gt;" u="1"/>
+        <s v="&lt;/jx:forEach&gt;" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Platform" numFmtId="0">
       <sharedItems containsBlank="1" count="2">
+        <s v="${g.platform}"/>
         <m/>
-        <s v="${g.platform}"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Description" numFmtId="0">
@@ -2215,19 +2294,18 @@
     </cacheField>
     <cacheField name="Weigh-in Time" numFmtId="49">
       <sharedItems containsBlank="1" count="2">
+        <s v="${g.weighInShortDateTime}"/>
         <m/>
-        <s v="${g.weighInShortDateTime}"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Start Time" numFmtId="49">
       <sharedItems containsBlank="1" count="2">
+        <s v="${g.competitionShortDateTime}"/>
         <m/>
-        <s v="${g.competitionShortDateTime}"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Role" numFmtId="0">
       <sharedItems containsBlank="1" count="18">
-        <m/>
         <s v="${t.get(&quot;Weighin1&quot;)}"/>
         <s v="${t.get(&quot;Weighin2&quot;)}"/>
         <s v="${t.get(&quot;Announcer&quot;)}"/>
@@ -2245,11 +2323,11 @@
         <s v="${t.get(&quot;Jury4&quot;)}"/>
         <s v="${t.get(&quot;Jury5&quot;)}"/>
         <s v="${t.get(&quot;Reserve&quot;)}"/>
+        <m/>
       </sharedItems>
     </cacheField>
     <cacheField name="Official" numFmtId="0">
       <sharedItems containsBlank="1" count="18">
-        <m/>
         <s v="${g.weighIn1}"/>
         <s v="${g.weighIn2}"/>
         <s v="${g.announcer}"/>
@@ -2267,6 +2345,7 @@
         <s v="${g.jury4}"/>
         <s v="${g.jury5}"/>
         <s v="${g.reserve}"/>
+        <m/>
       </sharedItems>
     </cacheField>
   </cacheFields>
@@ -2279,212 +2358,181 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="20">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="18">
   <r>
     <x v="0"/>
     <x v="0"/>
-    <m/>
+    <s v="${g.description}"/>
     <x v="0"/>
     <x v="0"/>
     <x v="0"/>
     <x v="0"/>
   </r>
   <r>
-    <x v="1"/>
-    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
     <s v="${g.description}"/>
-    <x v="1"/>
-    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
     <x v="1"/>
     <x v="1"/>
   </r>
   <r>
-    <x v="1"/>
-    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
     <s v="${g.description}"/>
-    <x v="1"/>
-    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
     <x v="2"/>
     <x v="2"/>
   </r>
   <r>
-    <x v="1"/>
-    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
     <s v="${g.description}"/>
-    <x v="1"/>
-    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
     <x v="3"/>
     <x v="3"/>
   </r>
   <r>
-    <x v="1"/>
-    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
     <s v="${g.description}"/>
-    <x v="1"/>
-    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
     <x v="4"/>
     <x v="4"/>
   </r>
   <r>
-    <x v="1"/>
-    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
     <s v="${g.description}"/>
-    <x v="1"/>
-    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
     <x v="5"/>
     <x v="5"/>
   </r>
   <r>
-    <x v="1"/>
-    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
     <s v="${g.description}"/>
-    <x v="1"/>
-    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
     <x v="6"/>
     <x v="6"/>
   </r>
   <r>
-    <x v="1"/>
-    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
     <s v="${g.description}"/>
-    <x v="1"/>
-    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
     <x v="7"/>
     <x v="7"/>
   </r>
   <r>
-    <x v="1"/>
-    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
     <s v="${g.description}"/>
-    <x v="1"/>
-    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
     <x v="8"/>
     <x v="8"/>
   </r>
   <r>
-    <x v="1"/>
-    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
     <s v="${g.description}"/>
-    <x v="1"/>
-    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
     <x v="9"/>
     <x v="9"/>
   </r>
   <r>
-    <x v="1"/>
-    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
     <s v="${g.description}"/>
-    <x v="1"/>
-    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
     <x v="10"/>
     <x v="10"/>
   </r>
   <r>
-    <x v="1"/>
-    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
     <s v="${g.description}"/>
-    <x v="1"/>
-    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
     <x v="11"/>
     <x v="11"/>
   </r>
   <r>
-    <x v="1"/>
-    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
     <s v="${g.description}"/>
-    <x v="1"/>
-    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
     <x v="12"/>
     <x v="12"/>
   </r>
   <r>
-    <x v="1"/>
-    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
     <s v="${g.description}"/>
-    <x v="1"/>
-    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
     <x v="13"/>
     <x v="13"/>
   </r>
   <r>
-    <x v="1"/>
-    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
     <s v="${g.description}"/>
-    <x v="1"/>
-    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
     <x v="14"/>
     <x v="14"/>
   </r>
   <r>
-    <x v="1"/>
-    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
     <s v="${g.description}"/>
-    <x v="1"/>
-    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
     <x v="15"/>
     <x v="15"/>
   </r>
   <r>
-    <x v="1"/>
-    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
     <s v="${g.description}"/>
-    <x v="1"/>
-    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
     <x v="16"/>
     <x v="16"/>
   </r>
   <r>
     <x v="1"/>
     <x v="1"/>
-    <s v="${g.description}"/>
+    <m/>
     <x v="1"/>
     <x v="1"/>
     <x v="17"/>
     <x v="17"/>
   </r>
-  <r>
-    <x v="2"/>
-    <x v="0"/>
-    <m/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="0"/>
-    <m/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable2" cacheId="19" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Data" updatedVersion="8" minRefreshableVersion="3" showMemberPropertyTips="0" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" gridDropZones="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable2" cacheId="9" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Data" updatedVersion="8" minRefreshableVersion="3" showMemberPropertyTips="0" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" gridDropZones="1">
   <location ref="A3:L22" firstHeaderRow="2" firstDataRow="2" firstDataCol="6"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" includeNewItemsInFilter="1" defaultSubtotal="0">
       <items count="4">
-        <item x="1"/>
-        <item x="2"/>
         <item x="0"/>
-        <item x="3"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" includeNewItemsInFilter="1" defaultSubtotal="0">
-      <items count="2">
-        <item x="1"/>
-        <item x="0"/>
-      </items>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" includeNewItemsInFilter="1"/>
-    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" includeNewItemsInFilter="1" defaultSubtotal="0">
-      <items count="2">
-        <item x="0"/>
+        <item m="1" x="3"/>
+        <item m="1" x="2"/>
         <item x="1"/>
       </items>
     </pivotField>
@@ -2494,8 +2542,22 @@
         <item x="1"/>
       </items>
     </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" includeNewItemsInFilter="1"/>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" includeNewItemsInFilter="1" defaultSubtotal="0">
+      <items count="2">
+        <item x="1"/>
+        <item x="0"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" includeNewItemsInFilter="1" defaultSubtotal="0">
+      <items count="2">
+        <item x="1"/>
+        <item x="0"/>
+      </items>
+    </pivotField>
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" includeNewItemsInFilter="1" defaultSubtotal="0">
       <items count="18">
+        <item x="17"/>
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
@@ -2513,12 +2575,12 @@
         <item x="14"/>
         <item x="15"/>
         <item x="16"/>
-        <item x="17"/>
       </items>
     </pivotField>
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" includeNewItemsInFilter="1" defaultSubtotal="0">
       <items count="18">
-        <item h="1" x="0"/>
+        <item h="1" x="17"/>
+        <item x="0"/>
         <item x="1"/>
         <item x="2"/>
         <item x="3"/>
@@ -2535,7 +2597,6 @@
         <item x="14"/>
         <item x="15"/>
         <item x="16"/>
-        <item x="17"/>
       </items>
     </pivotField>
   </pivotFields>
@@ -3324,7 +3385,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" workbookViewId="0">
       <pane xSplit="5" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A10" sqref="A10"/>
+      <selection pane="topRight" activeCell="C11" sqref="C11:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -3348,7 +3409,7 @@
   <sheetData>
     <row r="1" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="24"/>
@@ -3356,7 +3417,7 @@
         <v>12</v>
       </c>
       <c r="F1" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G1" s="13"/>
       <c r="H1" s="13"/>
@@ -3366,7 +3427,7 @@
         <v>15</v>
       </c>
       <c r="M1" s="64" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N1" s="67"/>
       <c r="P1" s="22"/>
@@ -3376,14 +3437,14 @@
     </row>
     <row r="2" spans="1:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="19"/>
       <c r="E2" s="26" t="s">
         <v>16</v>
       </c>
       <c r="F2" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G2" s="13"/>
       <c r="H2" s="13"/>
@@ -3393,14 +3454,14 @@
     </row>
     <row r="3" spans="1:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="21"/>
       <c r="E3" s="26" t="s">
         <v>13</v>
       </c>
       <c r="F3" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
@@ -3411,14 +3472,14 @@
     </row>
     <row r="4" spans="1:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" s="20"/>
       <c r="E4" s="26" t="s">
         <v>14</v>
       </c>
       <c r="F4" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G4" s="13"/>
       <c r="H4" s="13"/>
@@ -3430,7 +3491,7 @@
     <row r="5" spans="1:22" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:22" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="68" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B6" s="68"/>
       <c r="C6" s="68"/>
@@ -3512,7 +3573,7 @@
         <v>6</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K9" s="10" t="s">
         <v>4</v>
@@ -3521,25 +3582,25 @@
         <v>3</v>
       </c>
       <c r="M9" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="N9" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="N9" s="10" t="s">
-        <v>82</v>
-      </c>
       <c r="O9" s="10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="P9" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q9" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="R9" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="Q9" s="10" t="s">
+      <c r="S9" s="10" t="s">
         <v>107</v>
-      </c>
-      <c r="R9" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="S9" s="10" t="s">
-        <v>109</v>
       </c>
       <c r="T9" s="10" t="s">
         <v>1</v>
@@ -3548,75 +3609,75 @@
         <v>2</v>
       </c>
       <c r="V9" s="12" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:22" s="40" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="C10" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="D10" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="30" t="s">
+      <c r="E10" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="43" t="s">
+        <v>115</v>
+      </c>
+      <c r="G10" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="H10" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="I10" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="J10" s="41" t="s">
+        <v>114</v>
+      </c>
+      <c r="K10" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="L10" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="M10" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="N10" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="O10" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="P10" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q10" s="42" t="s">
+        <v>108</v>
+      </c>
+      <c r="R10" s="42" t="s">
+        <v>109</v>
+      </c>
+      <c r="S10" s="42" t="s">
+        <v>110</v>
+      </c>
+      <c r="T10" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="43" t="s">
-        <v>117</v>
-      </c>
-      <c r="G10" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="H10" s="34" t="s">
-        <v>104</v>
-      </c>
-      <c r="I10" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="J10" s="41" t="s">
-        <v>116</v>
-      </c>
-      <c r="K10" s="39" t="s">
-        <v>38</v>
-      </c>
-      <c r="L10" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="M10" s="42" t="s">
-        <v>81</v>
-      </c>
-      <c r="N10" s="42" t="s">
-        <v>83</v>
-      </c>
-      <c r="O10" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="P10" s="42" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q10" s="42" t="s">
-        <v>110</v>
-      </c>
-      <c r="R10" s="42" t="s">
+      <c r="U10" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="V10" s="42" t="s">
         <v>111</v>
-      </c>
-      <c r="S10" s="42" t="s">
-        <v>112</v>
-      </c>
-      <c r="T10" s="32" t="s">
-        <v>27</v>
-      </c>
-      <c r="U10" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="V10" s="42" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
@@ -7204,8 +7265,8 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:V5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="5" topLeftCell="F1" activePane="topRight" state="frozen"/>
@@ -7233,154 +7294,136 @@
         <v>3</v>
       </c>
       <c r="B2" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="H2" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="I2" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="J2" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="K2" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="L2" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="M2" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="N2" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="36" t="s">
-        <v>86</v>
-      </c>
-      <c r="D2" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="E2" s="36" t="s">
-        <v>79</v>
-      </c>
-      <c r="F2" s="36" t="s">
-        <v>76</v>
-      </c>
-      <c r="G2" s="36" t="s">
-        <v>77</v>
-      </c>
-      <c r="H2" s="36" t="s">
-        <v>74</v>
-      </c>
-      <c r="I2" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="J2" s="36" t="s">
-        <v>90</v>
-      </c>
-      <c r="K2" s="36" t="s">
-        <v>73</v>
-      </c>
-      <c r="L2" s="36" t="s">
+      <c r="O2" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="P2" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="M2" s="36" t="s">
-        <v>88</v>
-      </c>
-      <c r="N2" s="36" t="s">
-        <v>63</v>
-      </c>
-      <c r="O2" s="36" t="s">
+      <c r="Q2" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="R2" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="P2" s="36" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q2" s="36" t="s">
+      <c r="S2" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="R2" s="36" t="s">
+      <c r="T2" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="S2" s="36" t="s">
+      <c r="U2" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="T2" s="36" t="s">
-        <v>69</v>
-      </c>
-      <c r="U2" s="36" t="s">
+      <c r="V2" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="V2" s="36" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    </row>
+    <row r="3" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D3"/>
-      <c r="E3" s="1"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-    </row>
-    <row r="4" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="C3" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="E3" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="F3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D4" s="37" t="s">
-        <v>44</v>
-      </c>
-      <c r="E4" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="K4" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="M4" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="N4" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="R3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="V3" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="Q4" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5"/>
-      <c r="E5"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -7388,6 +7431,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -7416,7 +7460,7 @@
   <sheetData>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="47" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -7435,22 +7479,22 @@
     </row>
     <row r="4" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="61" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" s="49" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="D4" s="49" t="s">
+        <v>92</v>
+      </c>
+      <c r="E4" s="49" t="s">
         <v>93</v>
       </c>
-      <c r="B4" s="49" t="s">
-        <v>96</v>
-      </c>
-      <c r="C4" s="49" t="s">
-        <v>98</v>
-      </c>
-      <c r="D4" s="49" t="s">
-        <v>94</v>
-      </c>
-      <c r="E4" s="49" t="s">
-        <v>95</v>
-      </c>
       <c r="F4" s="49" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G4" s="54"/>
       <c r="H4" s="53"/>
@@ -7461,22 +7505,22 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="60" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D5" s="50" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E5" s="50" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F5" s="50" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G5" s="50"/>
       <c r="H5" s="51"/>
@@ -7487,22 +7531,22 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="60" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D6" s="50" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E6" s="50" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F6" s="50" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G6" s="54"/>
       <c r="H6" s="53"/>
@@ -7513,22 +7557,22 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="60" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C7" s="50" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D7" s="50" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E7" s="50" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F7" s="50" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G7" s="54"/>
       <c r="H7" s="53"/>
@@ -7539,22 +7583,22 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="60" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B8" s="50" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C8" s="50" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D8" s="50" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E8" s="50" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F8" s="50" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G8" s="54"/>
       <c r="H8" s="53"/>
@@ -7565,22 +7609,22 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="60" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B9" s="50" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C9" s="50" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D9" s="50" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E9" s="50" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F9" s="50" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G9" s="54"/>
       <c r="H9" s="53"/>
@@ -7591,22 +7635,22 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="60" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B10" s="50" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C10" s="50" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D10" s="50" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E10" s="50" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F10" s="50" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G10" s="54"/>
       <c r="H10" s="53"/>
@@ -7617,22 +7661,22 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="60" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B11" s="50" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C11" s="50" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D11" s="50" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E11" s="50" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F11" s="50" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G11" s="54"/>
       <c r="H11" s="53"/>
@@ -7643,22 +7687,22 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="60" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B12" s="50" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C12" s="50" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D12" s="50" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E12" s="50" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F12" s="50" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G12" s="54"/>
       <c r="H12" s="53"/>
@@ -7669,22 +7713,22 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="60" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B13" s="50" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C13" s="50" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D13" s="50" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E13" s="50" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F13" s="50" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G13" s="54"/>
       <c r="H13" s="53"/>
@@ -7695,22 +7739,22 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="60" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B14" s="50" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C14" s="50" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D14" s="50" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E14" s="50" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F14" s="50" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G14" s="54"/>
       <c r="H14" s="53"/>
@@ -7721,22 +7765,22 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="60" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B15" s="50" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C15" s="50" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D15" s="50" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E15" s="50" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F15" s="50" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G15" s="54"/>
       <c r="H15" s="53"/>
@@ -7747,22 +7791,22 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="60" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B16" s="50" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C16" s="50" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D16" s="50" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E16" s="50" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F16" s="50" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G16" s="54"/>
       <c r="H16" s="53"/>
@@ -7773,22 +7817,22 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="60" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B17" s="50" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C17" s="50" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D17" s="50" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E17" s="50" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F17" s="50" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G17" s="54"/>
       <c r="H17" s="53"/>
@@ -7799,22 +7843,22 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="60" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B18" s="50" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C18" s="50" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D18" s="50" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E18" s="50" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F18" s="50" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G18" s="54"/>
       <c r="H18" s="53"/>
@@ -7825,22 +7869,22 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="60" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B19" s="50" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C19" s="50" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D19" s="50" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E19" s="50" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F19" s="50" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G19" s="54"/>
       <c r="H19" s="53"/>
@@ -7851,22 +7895,22 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="60" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B20" s="50" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C20" s="50" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D20" s="50" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E20" s="50" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F20" s="50" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G20" s="54"/>
       <c r="H20" s="53"/>
@@ -7877,22 +7921,22 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="60" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B21" s="50" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C21" s="50" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D21" s="50" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E21" s="50" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F21" s="50" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G21" s="54"/>
       <c r="H21" s="53"/>
@@ -7903,7 +7947,7 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="62" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B22" s="63"/>
       <c r="C22" s="63"/>
@@ -7975,12 +8019,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:J602"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:J600"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A602" sqref="A602"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7996,54 +8038,74 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="36" t="s">
-        <v>98</v>
-      </c>
       <c r="C1" s="36" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1" s="44" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1" s="36" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="46" t="s">
         <v>99</v>
       </c>
-      <c r="D1" s="44" t="s">
-        <v>94</v>
-      </c>
-      <c r="E1" s="44" t="s">
-        <v>95</v>
-      </c>
-      <c r="F1" s="36" t="s">
-        <v>92</v>
-      </c>
-      <c r="G1" s="36" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2" s="46"/>
+      <c r="E2" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="F2" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="14"/>
+      <c r="I2"/>
+      <c r="J2"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D3" s="46" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E3" s="46" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F3" s="36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H3" s="14"/>
       <c r="I3"/>
@@ -8051,25 +8113,25 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D4" s="46" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E4" s="46" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F4" s="36" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H4" s="14"/>
       <c r="I4"/>
@@ -8077,25 +8139,25 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D5" s="46" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E5" s="46" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F5" s="36" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H5" s="14"/>
       <c r="I5"/>
@@ -8103,25 +8165,25 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D6" s="46" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E6" s="46" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F6" s="36" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>49</v>
+        <v>89</v>
       </c>
       <c r="H6" s="14"/>
       <c r="I6"/>
@@ -8129,51 +8191,51 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D7" s="46" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E7" s="46" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F7" s="36" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>91</v>
+        <v>48</v>
       </c>
       <c r="H7" s="14"/>
       <c r="I7"/>
       <c r="J7"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D8" s="46" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E8" s="46" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F8" s="36" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H8" s="14"/>
       <c r="I8"/>
@@ -8181,51 +8243,51 @@
     </row>
     <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="E9" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="F9" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="D9" s="46" t="s">
-        <v>101</v>
-      </c>
-      <c r="E9" s="46" t="s">
-        <v>102</v>
-      </c>
-      <c r="F9" s="36" t="s">
-        <v>62</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="H9" s="14"/>
       <c r="I9"/>
       <c r="J9"/>
     </row>
-    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D10" s="46" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E10" s="46" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F10" s="36" t="s">
-        <v>88</v>
+        <v>61</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>89</v>
+        <v>50</v>
       </c>
       <c r="H10" s="14"/>
       <c r="I10"/>
@@ -8233,25 +8295,25 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D11" s="46" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E11" s="46" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F11" s="36" t="s">
         <v>63</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H11" s="14"/>
       <c r="I11"/>
@@ -8259,25 +8321,25 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D12" s="46" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E12" s="46" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F12" s="36" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H12" s="14"/>
       <c r="I12"/>
@@ -8285,25 +8347,25 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D13" s="46" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E13" s="46" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F13" s="36" t="s">
         <v>64</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H13" s="14"/>
       <c r="I13"/>
@@ -8311,22 +8373,22 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D14" s="46" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E14" s="46" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F14" s="36" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>55</v>
@@ -8337,25 +8399,25 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D15" s="46" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E15" s="46" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F15" s="36" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H15" s="14"/>
       <c r="I15"/>
@@ -8363,25 +8425,25 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D16" s="46" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E16" s="46" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F16" s="36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H16" s="14"/>
       <c r="I16"/>
@@ -8389,25 +8451,25 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D17" s="46" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E17" s="46" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F17" s="36" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H17" s="14"/>
       <c r="I17"/>
@@ -8415,68 +8477,38 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D18" s="46" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E18" s="46" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F18" s="36" t="s">
         <v>70</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="H18" s="14"/>
-      <c r="I18"/>
       <c r="J18"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D19" s="46" t="s">
+    <row r="600" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A600" t="s">
         <v>101</v>
-      </c>
-      <c r="E19" s="46" t="s">
-        <v>102</v>
-      </c>
-      <c r="F19" s="36" t="s">
-        <v>72</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H19" s="14"/>
-      <c r="J19"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="602" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A602" t="s">
-        <v>103</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>